<commit_message>
data: add 2023-04-14 notices
</commit_message>
<xml_diff>
--- a/data/position_notices/2023-04-14.xlsx
+++ b/data/position_notices/2023-04-14.xlsx
@@ -466,39 +466,39 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>股票名称</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>股票代码</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>公告标题</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>公告日期</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>公告发布时间</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>公告链接</t>
         </is>
@@ -530,7 +530,7 @@
           <t>2023-04-14 18:13:51:000</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>https://data.eastmoney.com/notices/detail/002008/AN202304141585468163.html</t>
         </is>
@@ -562,7 +562,7 @@
           <t>2023-04-14 15:44:03:000</t>
         </is>
       </c>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>https://data.eastmoney.com/notices/detail/603109/AN202304141585460537.html</t>
         </is>
@@ -594,7 +594,7 @@
           <t>2023-04-14 17:39:57:000</t>
         </is>
       </c>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>https://data.eastmoney.com/notices/detail/000889/AN202304141585466753.html</t>
         </is>
@@ -626,7 +626,7 @@
           <t>2023-04-14 16:23:43:000</t>
         </is>
       </c>
-      <c r="F5" s="2" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>https://data.eastmoney.com/notices/detail/600887/AN202304141585462393.html</t>
         </is>
@@ -658,7 +658,7 @@
           <t>2023-04-14 16:23:43:000</t>
         </is>
       </c>
-      <c r="F6" s="2" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>https://data.eastmoney.com/notices/detail/002624/AN202304141585462394.html</t>
         </is>
@@ -690,7 +690,7 @@
           <t>2023-04-14 17:23:41:000</t>
         </is>
       </c>
-      <c r="F7" s="2" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>https://data.eastmoney.com/notices/detail/603007/AN202304141585466151.html</t>
         </is>
@@ -722,23 +722,14 @@
           <t>2023-04-14 17:23:41:000</t>
         </is>
       </c>
-      <c r="F8" s="2" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>https://data.eastmoney.com/notices/detail/603007/AN202304141585466150.html</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F3" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F4" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F7" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F8" r:id="rId7"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 

</xml_diff>